<commit_message>
additional fields timeframe and pointsdiff
additional fields timeframe and pointsdiff
</commit_message>
<xml_diff>
--- a/Statistic/Example.xlsx
+++ b/Statistic/Example.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\04_github\AgenaTrader\Statistic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Instrument</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Name of the strategy</t>
+  </si>
+  <si>
+    <t>TimeFrame</t>
+  </si>
+  <si>
+    <t>15M</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>PointsDiff</t>
   </si>
 </sst>
 </file>
@@ -188,7 +203,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -204,7 +219,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -500,25 +515,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="15" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="1"/>
+    <col min="17" max="18" width="9.1796875" style="1"/>
+    <col min="19" max="19" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -526,52 +541,58 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -579,50 +600,57 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>9500</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>9550</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>50</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>15</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>750</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
+        <f>H2-I2</f>
+        <v>-50</v>
+      </c>
+      <c r="O2" s="2">
         <v>9025</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3" t="b">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="b">
+      <c r="R2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -630,50 +658,57 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>9600</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>9580</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>-20</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>15</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>300</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:N5" si="0">H3-I3</f>
+        <v>20</v>
+      </c>
+      <c r="O3" s="2">
         <v>10080</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3" t="b">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="P3" s="3" t="b">
+      <c r="R3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -681,52 +716,59 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>9500</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>9550</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>50</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>15</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>750</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>-50</v>
+      </c>
+      <c r="O4" s="2">
         <v>9025</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>9550</v>
-      </c>
-      <c r="O4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3" t="b">
-        <v>0</v>
       </c>
       <c r="Q4" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -734,316 +776,351 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>9600</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>9580</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>-20</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>15</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>300</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="O5" s="2">
         <v>10080</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>9580</v>
-      </c>
-      <c r="O5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="3" t="b">
-        <v>0</v>
       </c>
       <c r="Q5" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
       <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
       <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
       <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
       <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
       <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
       <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
       <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
       <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
       <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
       <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
       <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1059,54 +1136,54 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>

</xml_diff>